<commit_message>
item import sample file updated
</commit_message>
<xml_diff>
--- a/public/files/import/items.xlsx
+++ b/public/files/import/items.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-8014\htdocs\v3\ak-modules2\public\files\import\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
     <sheet name="item_taxes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -46,26 +41,32 @@
     <t>Test item</t>
   </si>
   <si>
+    <t>service</t>
+  </si>
+  <si>
     <t>General</t>
   </si>
   <si>
+    <t>FALSE</t>
+  </si>
+  <si>
     <t>item_name</t>
   </si>
   <si>
     <t>tax_rate</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -74,21 +75,351 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -96,25 +427,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -401,26 +1017,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" customWidth="1"/>
+    <col min="1" max="2" width="11.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="17.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="16.4444444444444" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -451,7 +1067,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -460,31 +1076,16 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type Error" error="You must choose either product or service." sqref="B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type Error" error="You must choose either product or service." sqref="A3:A1048576;B2:B1048576">
       <formula1>"product,service"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enabled Error" error="You must choose either true or false." sqref="G2:G1048576">
@@ -492,182 +1093,45 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="1" max="2" width="10.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="str">
-        <f>IF(items!A2&lt;&gt;"",items!A2,"")</f>
-        <v>Test item</v>
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="str">
-        <f>IF(items!A3&lt;&gt;"",items!A3,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="str">
-        <f>IF(items!A4&lt;&gt;"",items!A4,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="str">
-        <f>IF(items!A5&lt;&gt;"",items!A5,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="str">
-        <f>IF(items!A6&lt;&gt;"",items!A6,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="str">
-        <f>IF(items!A7&lt;&gt;"",items!A7,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="str">
-        <f>IF(items!A8&lt;&gt;"",items!A8,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="str">
-        <f>IF(items!A9&lt;&gt;"",items!A9,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="str">
-        <f>IF(items!A10&lt;&gt;"",items!A10,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="str">
-        <f>IF(items!A11&lt;&gt;"",items!A11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="str">
-        <f>IF(items!A12&lt;&gt;"",items!A12,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="str">
-        <f>IF(items!A13&lt;&gt;"",items!A13,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="str">
-        <f>IF(items!A14&lt;&gt;"",items!A14,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="str">
-        <f>IF(items!A15&lt;&gt;"",items!A15,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="str">
-        <f>IF(items!A16&lt;&gt;"",items!A16,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="str">
-        <f>IF(items!A17&lt;&gt;"",items!A17,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="str">
-        <f>IF(items!A18&lt;&gt;"",items!A18,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="str">
-        <f>IF(items!A19&lt;&gt;"",items!A19,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="str">
-        <f>IF(items!A20&lt;&gt;"",items!A20,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="str">
-        <f>IF(items!A21&lt;&gt;"",items!A21,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="str">
-        <f>IF(items!A22&lt;&gt;"",items!A22,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="str">
-        <f>IF(items!A23&lt;&gt;"",items!A23,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="str">
-        <f>IF(items!A24&lt;&gt;"",items!A24,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="str">
-        <f>IF(items!A25&lt;&gt;"",items!A25,"")</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved items import file
</commit_message>
<xml_diff>
--- a/public/files/import/items.xlsx
+++ b/public/files/import/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
+    <workbookView windowWidth="17610" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -38,16 +38,19 @@
     <t>enabled</t>
   </si>
   <si>
-    <t>Test item</t>
+    <t>Test item 1</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Test item 2</t>
   </si>
   <si>
     <t>service</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
   <si>
     <t>item_name</t>
@@ -61,10 +64,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -82,43 +85,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,23 +124,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,18 +162,25 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -202,6 +191,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -211,15 +207,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,43 +237,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,13 +381,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,61 +399,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,55 +417,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,10 +433,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -450,15 +451,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,6 +479,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -498,6 +501,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,160 +528,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1023,19 +1026,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="2" width="11.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.8888888888889" customWidth="1"/>
-    <col min="5" max="5" width="17.5555555555556" customWidth="1"/>
-    <col min="6" max="6" width="16.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="12.8857142857143" customWidth="1"/>
+    <col min="5" max="5" width="17.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="16.447619047619" customWidth="1"/>
     <col min="7" max="7" width="9.33333333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1078,17 +1081,34 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type Error" error="You must choose either product or service." sqref="A3:A1048576;B2:B1048576">
-      <formula1>"product,service"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enabled Error" error="You must choose either true or false." sqref="G2:G1048576">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enabled Error" error="You must choose either true or false." sqref="G2 G3 G4:G1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1103,21 +1123,21 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="10.5555555555556" customWidth="1"/>
+    <col min="1" max="2" width="10.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>